<commit_message>
reading and writting data
</commit_message>
<xml_diff>
--- a/EPPlus4PHP.Test.PHP/test.xlsx
+++ b/EPPlus4PHP.Test.PHP/test.xlsx
@@ -8,72 +8,224 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\project\EPPlus4PHP\EPPlus4PHP.Test.PHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F2713BA-6BA8-45B5-857C-B6B36CD1FA57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A07F717-4830-4F70-9DF7-2E10263012F6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="9612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <t>d</t>
-    </r>
-    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <rPr>
-        <u val="singleAccounting"/>
-        <sz val="50"/>
-        <color rgb="FFBBCCDD"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>wadwa</t>
-    </r>
-    <phoneticPr xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>B14</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>B15</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>B16</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>B17</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>B18</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>B19</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>B20</t>
+  </si>
+  <si>
+    <t>C20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##,###"/>
-    <numFmt numFmtId="165" formatCode="yyyy/m/d h:mm"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <u val="singleAccounting"/>
-      <vertAlign val="superscript"/>
-      <sz val="50"/>
-      <color rgb="FFBBCCDD"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00BBCCDD" tint="0"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -81,28 +233,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left/>
-      <right/>
-      <top style="dotted">
-        <color rgb="00BBCCDD" tint="0"/>
-      </top>
-      <bottom style="dotted">
-        <color rgb="FF00FF00" tint="0"/>
-      </bottom>
-      <diagonal style="dashed">
-        <color rgb="FF0000FF" tint="0"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -417,24 +555,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="54.44140625" customWidth="1" style="2"/>
+    <col min="1" max="1" width="7.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="72.6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="88.8" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>